<commit_message>
added total amount to sales report printing
</commit_message>
<xml_diff>
--- a/salesReport/sales_report.xlsx
+++ b/salesReport/sales_report.xlsx
@@ -327,18 +327,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Fastrack Streetline 3.0 Analog-Digital Watch ver 1.0</v>
+        <v>Item</v>
       </c>
-      <c r="B1">
-        <v>2538</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>Fastrack Streetline 3.0 Analog-Digital Watch </v>
-      </c>
-      <c r="B2">
-        <v>2534</v>
+      <c r="B1" t="str">
+        <v>Total Amount Sold</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated convert excel file
</commit_message>
<xml_diff>
--- a/salesReport/sales_report.xlsx
+++ b/salesReport/sales_report.xlsx
@@ -15,7 +15,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,8 +23,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b>true</b>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="10"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none">
         <fgColor/>
@@ -37,8 +52,24 @@
         <bgColor/>
       </patternFill>
     </fill>
+    <fill/>
+    <fill/>
   </fills>
-  <borders count="1">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -50,8 +81,14 @@
   <cellStyleXfs count="1">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="false" applyNumberFormat="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFill="false" applyFont="true" applyNumberFormat="false" applyProtection="false" borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0">
+      <alignment/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="常规" xfId="0"/>
@@ -326,11 +363,35 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Item</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Total Amount Sold</v>
+      <c r="A1" s="1" t="str">
+        <v>Product</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <v>Amount Sold</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Fastrack Streetline 3.0 Analog-Digital Watch ver 1.0</v>
+      </c>
+      <c r="B2">
+        <v>2538</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Fastrack Streetline 3.0 Analog-Digital Watch </v>
+      </c>
+      <c r="B3">
+        <v>2534</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="str">
+        <v>Final Total</v>
+      </c>
+      <c r="B4" s="2">
+        <v>5072</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
orders error handling updated
</commit_message>
<xml_diff>
--- a/salesReport/sales_report.xlsx
+++ b/salesReport/sales_report.xlsx
@@ -372,26 +372,18 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Fastrack Streetline 3.0 Analog-Digital Watch ver 1.0</v>
+        <v>Fastrack Stunners 1.0</v>
       </c>
       <c r="B2">
-        <v>2538</v>
+        <v>12340.5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>Fastrack Streetline 3.0 Analog-Digital Watch </v>
-      </c>
-      <c r="B3">
-        <v>2534</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="str">
+      <c r="A3" s="2" t="str">
         <v>Final Total</v>
       </c>
-      <c r="B4" s="2">
-        <v>5072</v>
+      <c r="B3" s="2">
+        <v>12340.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>